<commit_message>
Generate maze using Randomized Prim's algorithm
</commit_message>
<xml_diff>
--- a/HoursLog.xlsx
+++ b/HoursLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amberwessels/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Repos\MazeGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{49F91033-96F3-7148-A020-201798871A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B13C114-8777-4A3F-BC81-44C011BA070A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="500" windowWidth="34620" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DTT Test Hour Log" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Subject</t>
   </si>
@@ -46,18 +46,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Example 1</t>
-  </si>
-  <si>
-    <t>Implementing …</t>
-  </si>
-  <si>
-    <t>Example 2</t>
-  </si>
-  <si>
-    <t>Had some issues with…</t>
   </si>
   <si>
     <t>Total amount of hours</t>
@@ -95,6 +83,34 @@
       <t xml:space="preserve"> 
 Fill in the number of hours that were required to complete the test. Please include every step you took during the process and include a detailed description of every step. Add reasoning on why you took certain decisions or applied specific techniques. We prefer quality over quantity so take your time with the test and the log.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup the Project </t>
+  </si>
+  <si>
+    <t>Setup the github repo and create an empty unity 3d Project</t>
+  </si>
+  <si>
+    <t>Feature 1: Setup Grid generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Create a button to trigger generation 
+* Create a Base prefab (Puzzle unit), in prefab set offset to the cube of 0.5 
+unit on Oy axis so that I can easily position cubes on bottom edge instead of center
+* Create a primitive script setup of 2D byte array representing the metadata for the maze ( 1 -&gt; create cube, 0 -&gt; will skip the cube) 
+* Created a simple function that would create the cubes based on array values ( for now just treat like it has only 1s so have a plane of cubes). This would allow me to visually debug the next steps.
+</t>
+  </si>
+  <si>
+    <t>Feature 1: Create the first iteration of the Maze</t>
+  </si>
+  <si>
+    <t>14/5/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Using the Randomized Prim's pseudo algorith from the provided wiki page created the first geneartion. 
+* For now did not bother with code quality, focused on the core generation.
+</t>
   </si>
 </sst>
 </file>
@@ -397,11 +413,11 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="31">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -420,14 +436,10 @@
     <xf numFmtId="49" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -436,6 +448,20 @@
     </xf>
     <xf numFmtId="49" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1706,328 +1732,360 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="6.5" style="1" customWidth="1"/>
-    <col min="7" max="251" width="6.5" customWidth="1"/>
+    <col min="1" max="1" width="24.765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.765625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="8.61328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.61328125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="6.4609375" style="1" customWidth="1"/>
+    <col min="7" max="251" width="6.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+    <row r="1" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="10"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:6" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
+    </row>
+    <row r="3" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="C4" s="16">
+        <v>45055</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="93" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="16">
+        <v>45055</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
-    </row>
-    <row r="3" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="16" t="s">
+      <c r="E5" s="18"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="49.2" x14ac:dyDescent="0.4">
+      <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="20">
         <v>2</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="17">
-        <v>3</v>
-      </c>
-      <c r="C4" s="18">
+      <c r="C6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="106.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A8" s="5"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="20">
+        <v>5</v>
+      </c>
+      <c r="C9" s="16">
         <v>42736</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="17">
-        <v>3</v>
-      </c>
-      <c r="C5" s="18">
-        <v>42736</v>
-      </c>
-      <c r="D5" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="17">
-        <v>5</v>
-      </c>
-      <c r="C6" s="18">
-        <v>42736</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="20"/>
+      <c r="E9" s="18" t="s">
+        <v>8</v>
+      </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="18"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="18"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="18"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="18"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="18"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="18"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="18"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="18"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="18"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="18"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="3"/>
+    <row r="29" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="14">
-        <f>SUMIF(E4:E28,"&lt;&gt;x",B4:B28)</f>
-        <v>6</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+    <row r="30" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="18"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+    <row r="31" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="18"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+    <row r="32" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="3"/>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
+    <row r="33" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="22">
+        <f>SUMIF(E4:E31,"&lt;&gt;x",B4:B31)</f>
+        <v>2.75</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add posibility to input exact sizes instead of relying on Slider
</commit_message>
<xml_diff>
--- a/HoursLog.xlsx
+++ b/HoursLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Repos\MazeGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CA4A54-8CC9-4EF5-829D-39915427E2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDC9461-995B-4738-A0F8-381E877A49C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Subject</t>
   </si>
@@ -152,6 +152,18 @@
   </si>
   <si>
     <t>Curently moving camera is instant which is distracting I decided to move it smoothly using lerping. Using as reference: https://gamedevbeginner.com/the-right-way-to-lerp-in-unity-with-examples/. I quickly made a small function using coroutines</t>
+  </si>
+  <si>
+    <t>Feature 3: Sizing limits</t>
+  </si>
+  <si>
+    <t>I have made several updates to the mazeSettings in order to prevent accidentally assigning excessively large values from Unity. Additionally, I have implemented additional checks in the setters to ensure proper validation. The view now utilizes a slider, and upon starting the application, I automatically set the minimum and maximum values to align with the sizing limits specified in MazeSettings</t>
+  </si>
+  <si>
+    <t>Feature  3: Improving the UX</t>
+  </si>
+  <si>
+    <t>Current slider does not show actual values, therefore user lacks controls. I decided to add 2 an extra text input where user can specify the  size more exactly.</t>
   </si>
 </sst>
 </file>
@@ -1777,10 +1789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1845,7 +1857,7 @@
       <c r="E4" s="18"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="121.2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="93" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1861,7 +1873,7 @@
       <c r="E5" s="18"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="42" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="49.2" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
@@ -1959,62 +1971,80 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
-      <c r="A12" s="5"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="26"/>
+    <row r="12" spans="1:6" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="A12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>31</v>
+      </c>
       <c r="E12" s="18"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>6</v>
+    <row r="13" spans="1:6" ht="25.2" x14ac:dyDescent="0.4">
+      <c r="A13" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="B13" s="20">
-        <v>5</v>
-      </c>
-      <c r="C13" s="16">
-        <v>42736</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>7</v>
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>33</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A14" s="5"/>
       <c r="B14" s="20"/>
       <c r="C14" s="16"/>
-      <c r="D14" s="14"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="18"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A15" s="5"/>
       <c r="B15" s="20"/>
       <c r="C15" s="16"/>
-      <c r="D15" s="14"/>
+      <c r="D15" s="26"/>
       <c r="E15" s="18"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A16" s="5"/>
       <c r="B16" s="20"/>
       <c r="C16" s="16"/>
-      <c r="D16" s="14"/>
+      <c r="D16" s="26"/>
       <c r="E16" s="18"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="18"/>
+      <c r="A17" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="20">
+        <v>5</v>
+      </c>
+      <c r="C17" s="16">
+        <v>42736</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>8</v>
+      </c>
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2161,50 +2191,82 @@
       <c r="E35" s="18"/>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="11"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="3"/>
+    <row r="36" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="18"/>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
+    <row r="37" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="5"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="11"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="22">
-        <f>SUMIF(E4:E35,"&lt;&gt;x",B4:B35)</f>
-        <v>6.75</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="6"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="6"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="4"/>
-    </row>
-    <row r="40" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="9"/>
+      <c r="B41" s="22">
+        <f>SUMIF(E4:E39,"&lt;&gt;x",B4:B39)</f>
+        <v>7.25</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Ensure that menu is completly closed
</commit_message>
<xml_diff>
--- a/HoursLog.xlsx
+++ b/HoursLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Repos\MazeGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614F17D1-E35D-4DAE-875F-94A22F0466E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E7F043-FCD3-47FA-9F67-12F54CC50B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Subject</t>
   </si>
@@ -136,16 +136,10 @@
     <t>Feature 2: See maze in entirety</t>
   </si>
   <si>
-    <t>18/05/2024</t>
-  </si>
-  <si>
     <t>To make sure the view includes the whole maze I created the functionality using right- triangle. The image in short showing the idea is in the Extra Folder, CameraDistanceImage.png. The Idea I got via googling but lost the link.</t>
   </si>
   <si>
     <t>Feature 2: Avoid camera jumping</t>
-  </si>
-  <si>
-    <t>18/05/2025</t>
   </si>
   <si>
     <t>X</t>
@@ -178,6 +172,14 @@
     <t>Since the Menu takes a significant chunck of screen I though it would be better to give the user possibility to collapse it.
 Quckly checked this tutorial to remind how masks work: https://learn.unity.com/tutorial/ui-masking#6032b6a4edbc2a33c1908e68. 
 The problem appeared with layouts, since layouts do not get recalculateds automatically if you resize chidlren. therefore had to use:  LayoutRebuilder.MarkLayoutForRebuild(layoutGroup);</t>
+  </si>
+  <si>
+    <t>Feature Extra: Animate the algorithm</t>
+  </si>
+  <si>
+    <t>I have added an additional task to implement animated maze generation.
+To accomplish this, I have created a new function that returns animation frames, represented as a boolean array per frame. Storing all the frames should not be a concern since the array is a byte array, which doesn't consume excessive memory.
+However, I noticed a previous issue where all prefabs were being deleted when creating a new maze. To address this problem and avoid excessive memory allocation and release, I have made some changes. Now, I create an object pool of prefabs based on the size of the first frame. These prefabs are initially disabled in the scene. During the animation, I simply enable or disable the prefabs based on whether they should represent a wall or a path in the frame.</t>
   </si>
 </sst>
 </file>
@@ -1803,10 +1805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1855,7 +1857,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:12" ht="16.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1960,128 +1962,140 @@
         <v>1</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>24</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>25</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:12" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="20">
         <v>1</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="26" t="s">
-        <v>29</v>
-      </c>
       <c r="E11" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" s="20">
         <v>0.5</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:12" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="20">
         <v>0.5</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:12" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" s="20">
         <v>0.5</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="93" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="109.2" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15" s="20">
         <v>1.5</v>
       </c>
-      <c r="C15" s="16"/>
+      <c r="C15" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="D15" s="26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="18"/>
+    <row r="16" spans="1:12" ht="157.19999999999999" x14ac:dyDescent="0.4">
+      <c r="A16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="20">
+        <v>1.25</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+    <row r="17" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="5"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="20">
+      <c r="B18" s="20">
         <v>5</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C18" s="16">
         <v>42736</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E18" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="18"/>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2252,30 +2266,30 @@
       <c r="E39" s="18"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="11"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="3"/>
+    <row r="40" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="5"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="18"/>
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="22">
-        <f>SUMIF(E4:E39,"&lt;&gt;x",B4:B39)</f>
-        <v>9.25</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
       <c r="E41" s="3"/>
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
-      <c r="B42" s="23"/>
+      <c r="A42" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="22">
+        <f>SUMIF(E4:E40,"&lt;&gt;x",B4:B40)</f>
+        <v>9.25</v>
+      </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
@@ -2290,12 +2304,20 @@
       <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="9"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Logs the time for second animation iteration
</commit_message>
<xml_diff>
--- a/HoursLog.xlsx
+++ b/HoursLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Repos\MazeGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E7F043-FCD3-47FA-9F67-12F54CC50B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4647A0B-69DA-4473-A96D-DB79E70A3C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Subject</t>
   </si>
@@ -177,9 +177,46 @@
     <t>Feature Extra: Animate the algorithm</t>
   </si>
   <si>
-    <t>I have added an additional task to implement animated maze generation.
+    <t>Feature Extra: Animate the algorithm iteration 2</t>
+  </si>
+  <si>
+    <t>19/05/2023</t>
+  </si>
+  <si>
+    <r>
+      <t>I Noticed that the animation statrted to negatively affect the Performance dropping from 30FPS when no animation is used to ~7FPS with animation. 
+My First Idea was to reduce number for loops ( since every frame was reading trough a 250x250 boolean array. For each step which sounded a bit too excesive. 
+So I desided to change the data stracture to use DeltaMazeAnimation. Where I just have a list of objects that have to be desable in the expected order of animation
+The Idea Iustrated in: Extra/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>MazeAnimSubractionVector2.jpg</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I have added an additional task to implement animated maze generation.
 To accomplish this, I have created a new function that returns animation frames, represented as a boolean array per frame. Storing all the frames should not be a concern since the array is a byte array, which doesn't consume excessive memory.
-However, I noticed a previous issue where all prefabs were being deleted when creating a new maze. To address this problem and avoid excessive memory allocation and release, I have made some changes. Now, I create an object pool of prefabs based on the size of the first frame. These prefabs are initially disabled in the scene. During the animation, I simply enable or disable the prefabs based on whether they should represent a wall or a path in the frame.</t>
+However, I noticed a previous issue where all prefabs were being deleted when creating a new maze. To address this problem and avoid excessive memory allocation and release, I have made some changes. Now, I create an object pool of prefabs based on the size of the first frame. These prefabs are initially disabled in the scene. During the animation, I simply enable or disable the prefabs based on whether they should represent a wall or a path in the frame.
+The illustration is in the file Extra/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>MazeAnimSubractionArray.jpg</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1805,10 +1842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2038,7 +2075,7 @@
       <c r="E14" s="18"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:12" ht="109.2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="93" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>34</v>
       </c>
@@ -2054,7 +2091,7 @@
       <c r="E15" s="18"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="157.19999999999999" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="181.2" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -2065,53 +2102,63 @@
         <v>21</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>26</v>
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="5"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="18"/>
+    <row r="17" spans="1:6" ht="133.19999999999999" x14ac:dyDescent="0.4">
+      <c r="A17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="20">
+        <v>1</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="20">
-        <v>5</v>
-      </c>
-      <c r="C18" s="16">
-        <v>42736</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>8</v>
-      </c>
+    <row r="18" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A18" s="5"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A19" s="5"/>
       <c r="B19" s="20"/>
       <c r="C19" s="16"/>
-      <c r="D19" s="14"/>
+      <c r="D19" s="26"/>
       <c r="E19" s="18"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="18"/>
+      <c r="A20" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="20">
+        <v>5</v>
+      </c>
+      <c r="C20" s="16">
+        <v>42736</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>8</v>
+      </c>
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2274,50 +2321,66 @@
       <c r="E40" s="18"/>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="3"/>
+    <row r="41" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="5"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="18"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="22">
-        <f>SUMIF(E4:E40,"&lt;&gt;x",B4:B40)</f>
-        <v>9.25</v>
-      </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+    <row r="42" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="5"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="18"/>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
       <c r="E43" s="3"/>
       <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="6"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="22">
+        <f>SUMIF(E4:E42,"&lt;&gt;x",B4:B42)</f>
+        <v>9.25</v>
+      </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="9"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
remove bool arrays for animation frames.
</commit_message>
<xml_diff>
--- a/HoursLog.xlsx
+++ b/HoursLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Repos\MazeGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4647A0B-69DA-4473-A96D-DB79E70A3C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502A2B69-103A-49E4-B448-E448300D77AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>Subject</t>
   </si>
@@ -217,6 +217,17 @@
       </rPr>
       <t>MazeAnimSubractionArray.jpg</t>
     </r>
+  </si>
+  <si>
+    <t>Feature Extra: Animate the algorithm optimization</t>
+  </si>
+  <si>
+    <t>20/05/2023</t>
+  </si>
+  <si>
+    <t>Removing extra arrays loops still affected the performance. 
+So I created a material and enabled GPU instancing  to reduce the batches count (Reducing from ~80k to 146)
+But it was not enough… stil ~10 FPS when animating.  I noticed using the porfiler, that there is a significant RAM of 3.5GB when animating vs 0.71GB when no animation is used. Turned out that I had a bug were I did not remove the chaching of the bool array steps, which in fact on a 250x250 maze would result in a significant memoy overhead. When I removed it I managed to get the RAM usage back to 0.71GB</t>
   </si>
 </sst>
 </file>
@@ -1845,7 +1856,7 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2091,7 +2102,7 @@
       <c r="E15" s="18"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="181.2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -2109,7 +2120,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="133.19999999999999" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="103.2" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
@@ -2127,12 +2138,22 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
-      <c r="A18" s="5"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="18"/>
+    <row r="18" spans="1:6" ht="121.2" x14ac:dyDescent="0.4">
+      <c r="A18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="20">
+        <v>1</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Create model to store AnimationFrames
</commit_message>
<xml_diff>
--- a/HoursLog.xlsx
+++ b/HoursLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Repos\MazeGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502A2B69-103A-49E4-B448-E448300D77AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8752C7-48B3-41CD-85AB-CE3DD806D657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>Subject</t>
   </si>
@@ -228,6 +228,27 @@
     <t>Removing extra arrays loops still affected the performance. 
 So I created a material and enabled GPU instancing  to reduce the batches count (Reducing from ~80k to 146)
 But it was not enough… stil ~10 FPS when animating.  I noticed using the porfiler, that there is a significant RAM of 3.5GB when animating vs 0.71GB when no animation is used. Turned out that I had a bug were I did not remove the chaching of the bool array steps, which in fact on a 250x250 maze would result in a significant memoy overhead. When I removed it I managed to get the RAM usage back to 0.71GB</t>
+  </si>
+  <si>
+    <t>Feature Extra: Animate Algorithm Iteration 3</t>
+  </si>
+  <si>
+    <r>
+      <t>The current State is Relatively good, by the end of animation the frame rate is ~35FPS, however it is not the case while the animation is actually playing, starting from  9FPS and gradually increaseing as less and less mazeSections are visible.
+Which is the downside of the Subraction approach. Instead I wanted to try using Addition approach. (Adding only the list of walls when the alhorithm says it is a wall)
+Idea Illustrated: 
+The illustration is in the file</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Extra/MazeAnimAdditionWalls.jpg</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1853,10 +1874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1938,7 +1959,7 @@
       <c r="E5" s="18"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="49.2" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
@@ -1970,7 +1991,7 @@
       <c r="E7" s="18"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="73.2" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1986,7 +2007,7 @@
       <c r="E8" s="18"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:12" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="37.200000000000003" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
@@ -2002,7 +2023,7 @@
       <c r="E9" s="18"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:12" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="37.200000000000003" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -2018,7 +2039,7 @@
       <c r="E10" s="18"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:12" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="49.2" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -2036,7 +2057,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="61.2" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -2052,7 +2073,7 @@
       <c r="E12" s="18"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="25.2" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
@@ -2070,7 +2091,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="25.2" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
@@ -2102,7 +2123,7 @@
       <c r="E15" s="18"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="144" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="181.2" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -2120,7 +2141,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="103.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="166.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
@@ -2143,7 +2164,7 @@
         <v>41</v>
       </c>
       <c r="B18" s="20">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>42</v>
@@ -2156,46 +2177,54 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
-      <c r="A19" s="5"/>
-      <c r="B19" s="20"/>
+    <row r="19" spans="1:6" ht="121.2" x14ac:dyDescent="0.4">
+      <c r="A19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="20">
+        <v>1</v>
+      </c>
       <c r="C19" s="16"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="18"/>
+      <c r="D19" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="20">
-        <v>5</v>
-      </c>
-      <c r="C20" s="16">
-        <v>42736</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>8</v>
-      </c>
+    <row r="20" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A20" s="5"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
       <c r="A21" s="5"/>
       <c r="B21" s="20"/>
       <c r="C21" s="16"/>
-      <c r="D21" s="14"/>
+      <c r="D21" s="26"/>
       <c r="E21" s="18"/>
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="18"/>
+      <c r="A22" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="20">
+        <v>5</v>
+      </c>
+      <c r="C22" s="16">
+        <v>42736</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>8</v>
+      </c>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -2358,50 +2387,66 @@
       <c r="E42" s="18"/>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="11"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="3"/>
+    <row r="43" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="5"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="18"/>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="22">
-        <f>SUMIF(E4:E42,"&lt;&gt;x",B4:B42)</f>
-        <v>9.25</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+    <row r="44" spans="1:6" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="5"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="18"/>
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="6"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="A45" s="11"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
       <c r="E45" s="3"/>
       <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="6"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="22">
+        <f>SUMIF(E4:E44,"&lt;&gt;x",B4:B44)</f>
+        <v>9.25</v>
+      </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="9"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Make the Animation dedicated class, and controls to play/pause the animation
</commit_message>
<xml_diff>
--- a/HoursLog.xlsx
+++ b/HoursLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Repos\MazeGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A5C62C-3BB2-4B84-AABA-F6FB46790871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C197B92-74E3-432F-A5F0-445149F93888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>Subject</t>
   </si>
@@ -254,8 +254,10 @@
     <t>Featurure Extra: Refactor and User Experience</t>
   </si>
   <si>
-    <t>Now As user I would like to get control over the speed of the animation while also being able to move back in animation or even rewind. 
-But to simplify the process I first have to refactor the code and make sure that there are no data structure diferences based on some obscure paramters</t>
+    <t xml:space="preserve">Now As user I would like to get control over the speed of the animation while also being able to move back in animation or even rewind. 
+But to simplify the process I first have to refactor the code and make sure that there are no data structure diferences based on some obscure paramters.
+So I decided to make an abtraction that will display each frame 
+</t>
   </si>
 </sst>
 </file>
@@ -1883,8 +1885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1966,7 +1968,7 @@
       <c r="E5" s="18"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="49.2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" ht="42" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
@@ -1998,7 +2000,7 @@
       <c r="E7" s="18"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="73.2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -2014,7 +2016,7 @@
       <c r="E8" s="18"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:12" ht="37.200000000000003" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
@@ -2030,7 +2032,7 @@
       <c r="E9" s="18"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:12" ht="37.200000000000003" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
@@ -2046,7 +2048,7 @@
       <c r="E10" s="18"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:12" ht="49.2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -2064,7 +2066,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:12" ht="61.2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -2080,7 +2082,7 @@
       <c r="E12" s="18"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="25.2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>30</v>
       </c>
@@ -2098,7 +2100,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:12" ht="25.2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>32</v>
       </c>
@@ -2130,7 +2132,7 @@
       <c r="E15" s="18"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:12" ht="181.2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="144" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>36</v>
       </c>
@@ -2166,7 +2168,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="121.2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="103.2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>41</v>
       </c>
@@ -2184,7 +2186,7 @@
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="133.19999999999999" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="113.4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>44</v>
       </c>
@@ -2202,19 +2204,23 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="61.2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="97.2" x14ac:dyDescent="0.4">
       <c r="A20" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="16"/>
+      <c r="B20" s="20">
+        <v>3</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="D20" s="26" t="s">
         <v>47</v>
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="20"/>
       <c r="C21" s="16"/>
@@ -2430,7 +2436,7 @@
       </c>
       <c r="B46" s="22">
         <f>SUMIF(E4:E44,"&lt;&gt;x",B4:B44)</f>
-        <v>9.25</v>
+        <v>12.25</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>

</xml_diff>

<commit_message>
Remove animation control with slider
</commit_message>
<xml_diff>
--- a/HoursLog.xlsx
+++ b/HoursLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Repos\MazeGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08606A9D-3324-4951-B872-4A68A3EE4F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E811D4B-4D36-4A97-893B-419ADB56884E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>Subject</t>
   </si>
@@ -266,6 +266,9 @@
     <t>Working on animation speed controls (like reverse/forward/ pause). 
 This could be perfect for debugging new algorithms.
 The whole time I was mainly focusing on creating the approprieate events, creating View scripts and expading the MazeAnimationClass to support the desired functionality</t>
+  </si>
+  <si>
+    <t>Debug rewind animation… Often animation frames where storing extra walls (not only delta which was causing during the rewind unexpected artifacts)</t>
   </si>
 </sst>
 </file>
@@ -1894,7 +1897,7 @@
   <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.4609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2248,12 +2251,22 @@
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">
-      <c r="A22" s="5"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="18"/>
+    <row r="22" spans="1:6" ht="25.2" x14ac:dyDescent="0.4">
+      <c r="A22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="20">
+        <v>5</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>26</v>
+      </c>
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.4">

</xml_diff>